<commit_message>
update validasi npm dan sorting prestasi berdasarkan jurusan
</commit_message>
<xml_diff>
--- a/public/akun-user/test.xlsx
+++ b/public/akun-user/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\.xlx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF805649-38DD-4865-B206-71FE4D53796A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E70C573-F34A-4203-9B3E-DE72DEB31C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B2A60AC3-26ED-4C30-A489-588FF12E2CC6}"/>
   </bookViews>
@@ -63,12 +63,6 @@
     <t>ngawi</t>
   </si>
   <si>
-    <t>Muhammad Irfan</t>
-  </si>
-  <si>
-    <t>G1A021082</t>
-  </si>
-  <si>
     <t>mirfan1312@gmail.com</t>
   </si>
   <si>
@@ -93,10 +87,16 @@
     <t>adsadas</t>
   </si>
   <si>
-    <t>G1A021099</t>
-  </si>
-  <si>
     <t>dfsdfs@gmail.com</t>
+  </si>
+  <si>
+    <t>H1A021099</t>
+  </si>
+  <si>
+    <t>Muhammad ssed</t>
+  </si>
+  <si>
+    <t>G1A021066</t>
   </si>
 </sst>
 </file>
@@ -462,7 +462,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -517,62 +517,62 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
       <c r="F4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>